<commit_message>
add some more audio
</commit_message>
<xml_diff>
--- a/data/audio/audio.xlsx
+++ b/data/audio/audio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{597A3B66-688B-454C-9315-CA31FFD93134}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CA644A5-E183-4506-8E2E-2056B0E35817}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>species_scientific_name</t>
   </si>
@@ -151,6 +151,90 @@
   </si>
   <si>
     <t>Nyngan, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/157488/download</t>
+  </si>
+  <si>
+    <t>Acanthiza pusilla</t>
+  </si>
+  <si>
+    <t>Noosa Heads, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Fernand Deroussen</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/UXGZWVYDFE</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-nd/3.0/</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/396904/download</t>
+  </si>
+  <si>
+    <t>Comerong Island, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Acanthiza reguloides</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/85990/download</t>
+  </si>
+  <si>
+    <t>Moggill State Forest, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Nick Leseberg</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/FWTRWUQQAA</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-nd/2.5/</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/365188/download</t>
+  </si>
+  <si>
+    <t>Nangar National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Acanthorhynchus tenuirostris</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/357302/download</t>
+  </si>
+  <si>
+    <t>Abercrombie Caves, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/209907/download</t>
+  </si>
+  <si>
+    <t>Accipiter cirrocephalus</t>
+  </si>
+  <si>
+    <t>Royal National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Accipiter fasciatus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/340225/download</t>
+  </si>
+  <si>
+    <t>Wollemi National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Accipiter novaehollandiae</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/434627/download</t>
+  </si>
+  <si>
+    <t>Eungella, Queensland, Australia</t>
   </si>
 </sst>
 </file>
@@ -509,15 +593,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:G9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
@@ -731,6 +815,190 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
whole bunch of xeno-canto audio
</commit_message>
<xml_diff>
--- a/data/audio/audio.xlsx
+++ b/data/audio/audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CA644A5-E183-4506-8E2E-2056B0E35817}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{03BD4EF0-FCD0-4EA5-9A66-B5622C4D7A99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="190">
   <si>
     <t>species_scientific_name</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Andrew Spencer</t>
   </si>
   <si>
-    <t>https://ebird.org/profile/OTA0Njc#_ga=2.171409699.2024991290.1527555887-657555911.1527555887</t>
-  </si>
-  <si>
     <t>assets/misc/copyright.png</t>
   </si>
   <si>
@@ -235,6 +232,369 @@
   </si>
   <si>
     <t>Eungella, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Acridotheres tristis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/331569/download</t>
+  </si>
+  <si>
+    <t>Earlwood, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://ebird.org/profile/OTA0Njc</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/187497/download</t>
+  </si>
+  <si>
+    <t>Brunswick, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>Nick Talbot</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/CCUCXWCPSW</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/429269/download</t>
+  </si>
+  <si>
+    <t>Almada, Setúbal, Portugal</t>
+  </si>
+  <si>
+    <t>Antonio Xeira</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/PJVICFDZGZ</t>
+  </si>
+  <si>
+    <t>Acrocephalus australis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/407740/download</t>
+  </si>
+  <si>
+    <t>Lake Wendouree, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>Frank Lambert</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/YTUXOCTUEM</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/340135/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/107971/download</t>
+  </si>
+  <si>
+    <t>Herdsman Lake, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>Matthias Feuersenger</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/HBPYQXTJEV</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/397386/download</t>
+  </si>
+  <si>
+    <t>Actitis hypoleucos</t>
+  </si>
+  <si>
+    <t>Plaiaundi Ecology Park, Basque Country, Spain</t>
+  </si>
+  <si>
+    <t>Itziar Gutiérrez</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/HMJIMVISCP</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/383688/download</t>
+  </si>
+  <si>
+    <t>Aegotheles cristatus</t>
+  </si>
+  <si>
+    <t>Mount Gibson Sanctuary, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/335532/download</t>
+  </si>
+  <si>
+    <t>Mutawintji National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/243484/download</t>
+  </si>
+  <si>
+    <t>Mungo National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Jeremy Hegge</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/XKXDFWNSPA</t>
+  </si>
+  <si>
+    <t>Ailuroedus crassirostris</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/195638/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/146088/download</t>
+  </si>
+  <si>
+    <t>Watagan National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Alectura lathami</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/389279/download</t>
+  </si>
+  <si>
+    <t>Dharug National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/96883/download</t>
+  </si>
+  <si>
+    <t>Tamborine National Park, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Patrik Åberg</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/BPSDQEOJWG</t>
+  </si>
+  <si>
+    <t>Alisterus scapularis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/434416/download</t>
+  </si>
+  <si>
+    <t>Benarkin State Forest, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/327334/download</t>
+  </si>
+  <si>
+    <t>Kambah, Australian Capital Territory, Australia</t>
+  </si>
+  <si>
+    <t>Amaurornis moluccana</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/355755/download</t>
+  </si>
+  <si>
+    <t>Dayboro, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Tom Tarrant</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/BWGNIOJXYX</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/EYDMHIJPXV</t>
+  </si>
+  <si>
+    <t>Pieter de Groot Boersma</t>
+  </si>
+  <si>
+    <t>Carrington, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/326946/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/410512/download</t>
+  </si>
+  <si>
+    <t>Foli, Halmahera, Indonesia</t>
+  </si>
+  <si>
+    <t>Ross Gallardy</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/FNIOJOZADD</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/151729/download</t>
+  </si>
+  <si>
+    <t>Weda, Central Halmahera, Indonesia</t>
+  </si>
+  <si>
+    <t>Mike Nelson</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/PWDLINYMKL</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-sa/3.0/</t>
+  </si>
+  <si>
+    <t>Anas castanea</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/340216/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/204392/download</t>
+  </si>
+  <si>
+    <t>South Bruny Island, Tasmania, Australia</t>
+  </si>
+  <si>
+    <t>Anas gracilis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/434176/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/152951/download</t>
+  </si>
+  <si>
+    <t>Kinleith, Waikato, New Zealand</t>
+  </si>
+  <si>
+    <t>Anas platyrhynchos (Domestic type)</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/437498/download</t>
+  </si>
+  <si>
+    <t>Grant County, Washington, United States</t>
+  </si>
+  <si>
+    <t>Bruce Lagerquist</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/JHFICMRVUX</t>
+  </si>
+  <si>
+    <t>Anas superciliosa</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/439626/download</t>
+  </si>
+  <si>
+    <t>Lakefield National Park, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/366858/download</t>
+  </si>
+  <si>
+    <t>Gulpa Island State Forest, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Anhinga novaehollandiae</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/436716/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/367826/download</t>
+  </si>
+  <si>
+    <t>Kyeemagh, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/165480/download</t>
+  </si>
+  <si>
+    <t>Lakefield, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/LWOEIVFOSZ</t>
+  </si>
+  <si>
+    <t>Henk Krajenbrink</t>
+  </si>
+  <si>
+    <t>Anous minutus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/431362/download</t>
+  </si>
+  <si>
+    <t>Arquipelago de Fernando de Noronha, Pernambuco, Brazil</t>
+  </si>
+  <si>
+    <t>Jayrson Araujo de Oliveira</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/LXKLWEDKEM</t>
+  </si>
+  <si>
+    <t>Anous stolidus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/172325/download</t>
+  </si>
+  <si>
+    <t>Michaelmas Cay, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/148686/download</t>
+  </si>
+  <si>
+    <t>Cocos Island, Rodrigues, Mauritius</t>
+  </si>
+  <si>
+    <t>Johannes Fischer</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/IFRLJBSAMX</t>
+  </si>
+  <si>
+    <t>Anthochaera carunculata</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/172254/download</t>
+  </si>
+  <si>
+    <t>Kings Plains National Park, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/355059/download</t>
+  </si>
+  <si>
+    <t>Anthochaera chrysoptera</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/331580/download</t>
+  </si>
+  <si>
+    <t>Anthus novaeseelandiae</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/384316/download</t>
+  </si>
+  <si>
+    <t>Kurnell, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Antigone rubicunda</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/286924/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/172083/download</t>
+  </si>
+  <si>
+    <t>Kakadu National Park, Northern Territory, Australia</t>
   </si>
 </sst>
 </file>
@@ -276,9 +636,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,20 +954,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="50.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="1025" width="12.140625"/>
   </cols>
@@ -636,62 +998,65 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -702,42 +1067,42 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -748,258 +1113,1155 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" t="s">
+        <v>176</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:G50">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
audio up to the end of a - some trickier species still missing
</commit_message>
<xml_diff>
--- a/data/audio/audio.xlsx
+++ b/data/audio/audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{03BD4EF0-FCD0-4EA5-9A66-B5622C4D7A99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8F95DFD5-9701-42AB-9D1D-834753CF282B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="256">
   <si>
     <t>species_scientific_name</t>
   </si>
@@ -595,6 +595,204 @@
   </si>
   <si>
     <t>Kakadu National Park, Northern Territory, Australia</t>
+  </si>
+  <si>
+    <t>Aprosmictus erythropterus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/354254/download</t>
+  </si>
+  <si>
+    <t>Apus pacificus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/352598/download</t>
+  </si>
+  <si>
+    <t>Cattana Wetlands, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/286311/download</t>
+  </si>
+  <si>
+    <t>Kiritappu, Hokkaido, Japan</t>
+  </si>
+  <si>
+    <t>Peter Boesman</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/OOECIWCSWV</t>
+  </si>
+  <si>
+    <t>Ardea alba</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/365950/download</t>
+  </si>
+  <si>
+    <t>Freemans Reach, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/431288/download</t>
+  </si>
+  <si>
+    <t>Reserva Natural Palmarí, Rio Javarí, Brazil</t>
+  </si>
+  <si>
+    <t>Jerome Fischer</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/JPBSNBUUEF</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/439287/download</t>
+  </si>
+  <si>
+    <t>Ardea pacifica</t>
+  </si>
+  <si>
+    <t>Chong Swamp, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Ardenna carneipes</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/424726/download</t>
+  </si>
+  <si>
+    <t>Lady Alice Island, Whangarei District, New Zealand</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/YHOCFQHBDL</t>
+  </si>
+  <si>
+    <t>David Boyle</t>
+  </si>
+  <si>
+    <t>Ardenna pacifica</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/113088/download</t>
+  </si>
+  <si>
+    <t>Wilson Island, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Simon Elliott</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/FFFADKCCII</t>
+  </si>
+  <si>
+    <t>Ardenna tenuirostris</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/177452/download</t>
+  </si>
+  <si>
+    <t>Phillip Island, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>Arenaria interpres</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/435117/download</t>
+  </si>
+  <si>
+    <t>Patrick Franke</t>
+  </si>
+  <si>
+    <t>Snaefellsness, Iceland</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/311155/download</t>
+  </si>
+  <si>
+    <t>Bundala Wetland, Sri Lanka</t>
+  </si>
+  <si>
+    <t>Artamus cinereus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/428464/download</t>
+  </si>
+  <si>
+    <t>Roebuck Plains Station, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/334914/download</t>
+  </si>
+  <si>
+    <t>Tibooburra, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Artamus cyanopterus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/354593/download</t>
+  </si>
+  <si>
+    <t>Artamus leucorynchus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/283305/download</t>
+  </si>
+  <si>
+    <t>Tuggerah, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/283304/download</t>
+  </si>
+  <si>
+    <t>Artamus minor</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/107836/download</t>
+  </si>
+  <si>
+    <t>Kalbarri National Park, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>Artamus personatus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/287053/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/407726/download</t>
+  </si>
+  <si>
+    <t>Artamus superciliosus</t>
+  </si>
+  <si>
+    <t>Mt Ida, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/393405/download</t>
+  </si>
+  <si>
+    <t>Eubalong, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/389388/download</t>
+  </si>
+  <si>
+    <t>Pitt Town Lagoon, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Aviceda subcristata</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/438827/download</t>
+  </si>
+  <si>
+    <t>Oyala-Thumotang National Park, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Kabupaten Raja Ampat, Papua Barat, Indonesia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/409476/download</t>
   </si>
 </sst>
 </file>
@@ -954,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,6 +2456,535 @@
         <v>13</v>
       </c>
     </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>192</v>
+      </c>
+      <c r="B59" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" t="s">
+        <v>198</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" t="s">
+        <v>205</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" t="s">
+        <v>210</v>
+      </c>
+      <c r="C63" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" t="s">
+        <v>213</v>
+      </c>
+      <c r="E63" t="s">
+        <v>212</v>
+      </c>
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>214</v>
+      </c>
+      <c r="B64" t="s">
+        <v>215</v>
+      </c>
+      <c r="C64" t="s">
+        <v>216</v>
+      </c>
+      <c r="D64" t="s">
+        <v>217</v>
+      </c>
+      <c r="E64" t="s">
+        <v>218</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" t="s">
+        <v>221</v>
+      </c>
+      <c r="D65" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E66" t="s">
+        <v>223</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>222</v>
+      </c>
+      <c r="B67" t="s">
+        <v>226</v>
+      </c>
+      <c r="C67" t="s">
+        <v>227</v>
+      </c>
+      <c r="D67" t="s">
+        <v>197</v>
+      </c>
+      <c r="E67" t="s">
+        <v>198</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>228</v>
+      </c>
+      <c r="B68" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" t="s">
+        <v>230</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>228</v>
+      </c>
+      <c r="B69" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" t="s">
+        <v>32</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>233</v>
+      </c>
+      <c r="B70" t="s">
+        <v>234</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" t="s">
+        <v>27</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71" t="s">
+        <v>236</v>
+      </c>
+      <c r="C71" t="s">
+        <v>237</v>
+      </c>
+      <c r="D71" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>235</v>
+      </c>
+      <c r="B72" t="s">
+        <v>238</v>
+      </c>
+      <c r="C72" t="s">
+        <v>237</v>
+      </c>
+      <c r="D72" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" t="s">
+        <v>32</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" t="s">
+        <v>240</v>
+      </c>
+      <c r="C73" t="s">
+        <v>241</v>
+      </c>
+      <c r="D73" t="s">
+        <v>89</v>
+      </c>
+      <c r="E73" t="s">
+        <v>90</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>242</v>
+      </c>
+      <c r="B74" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>31</v>
+      </c>
+      <c r="E74" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>245</v>
+      </c>
+      <c r="B75" t="s">
+        <v>244</v>
+      </c>
+      <c r="C75" t="s">
+        <v>246</v>
+      </c>
+      <c r="D75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E75" t="s">
+        <v>85</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
+        <v>247</v>
+      </c>
+      <c r="C76" t="s">
+        <v>248</v>
+      </c>
+      <c r="D76" t="s">
+        <v>26</v>
+      </c>
+      <c r="E76" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" t="s">
+        <v>249</v>
+      </c>
+      <c r="C77" t="s">
+        <v>250</v>
+      </c>
+      <c r="D77" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>251</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" t="s">
+        <v>253</v>
+      </c>
+      <c r="D78" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>251</v>
+      </c>
+      <c r="B79" t="s">
+        <v>255</v>
+      </c>
+      <c r="C79" t="s">
+        <v>254</v>
+      </c>
+      <c r="D79" t="s">
+        <v>132</v>
+      </c>
+      <c r="E79" t="s">
+        <v>133</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:G50">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
audio up to RTBC
</commit_message>
<xml_diff>
--- a/data/audio/audio.xlsx
+++ b/data/audio/audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8F95DFD5-9701-42AB-9D1D-834753CF282B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ADD72F77-7D36-4013-9ED4-2B58099E887E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="360">
   <si>
     <t>species_scientific_name</t>
   </si>
@@ -793,6 +793,318 @@
   </si>
   <si>
     <t>https://www.xeno-canto.org/409476/download</t>
+  </si>
+  <si>
+    <t>Biziura lobata</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/201462/download</t>
+  </si>
+  <si>
+    <t>Dunn's Swamp, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Bubulcus ibis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/393573/download</t>
+  </si>
+  <si>
+    <t>Maleny, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Burhinus grallarius</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/439120/download</t>
+  </si>
+  <si>
+    <t>Coen River, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/382911/download</t>
+  </si>
+  <si>
+    <t>Dryandra Woodland, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/174119/download</t>
+  </si>
+  <si>
+    <t>Stewart Creek Valley, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Butorides striata</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/359600/download</t>
+  </si>
+  <si>
+    <t>Sabah, Borneo, Malaysia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/210507/download</t>
+  </si>
+  <si>
+    <t>Tweed Heads, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Cacatua galerita</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/438828/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/380456/download</t>
+  </si>
+  <si>
+    <t>Long Point, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Cacatua sanguinea</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/407697/download</t>
+  </si>
+  <si>
+    <t>Lake Hattah, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/320990/download</t>
+  </si>
+  <si>
+    <t>Maffra, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>Cacatua tenuirostris</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/200313/download</t>
+  </si>
+  <si>
+    <t>Wyperfeld National Park, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/187680/download</t>
+  </si>
+  <si>
+    <t>Adelaide, South Australia, Australia</t>
+  </si>
+  <si>
+    <t>Cacomantis flabelliformis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/407773/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/382702/download</t>
+  </si>
+  <si>
+    <t>Cheynes Beach, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/140206/download</t>
+  </si>
+  <si>
+    <t>Barren Grounds, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Cacomantis pallidus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/389397/download</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/389393/download</t>
+  </si>
+  <si>
+    <t>Cacomantis variolosus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/287384/download</t>
+  </si>
+  <si>
+    <t>Barcoongere State Forest, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/201458/download</t>
+  </si>
+  <si>
+    <t>Calidris acuminata</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/107605/download</t>
+  </si>
+  <si>
+    <t>St Paul Island, Alaska, United States</t>
+  </si>
+  <si>
+    <t>Ryan O'Donnell</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/SDXVTLDNGJ</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/283313/download</t>
+  </si>
+  <si>
+    <t>Calidris alba</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/412103/download</t>
+  </si>
+  <si>
+    <t>Orog Lake, Mongolia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/223302/download</t>
+  </si>
+  <si>
+    <t>Tarifa, Andalusia, Spain</t>
+  </si>
+  <si>
+    <t>Karri Kuitunen</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/XJIOOFMPPX</t>
+  </si>
+  <si>
+    <t>Calidris canutus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/416902/download</t>
+  </si>
+  <si>
+    <t>Balsnes, Troms, Norway</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/TLPLNAINFU</t>
+  </si>
+  <si>
+    <t>Stein Ø. Nilsen</t>
+  </si>
+  <si>
+    <t>Calidris falcinellus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/342360/download</t>
+  </si>
+  <si>
+    <t>Iisakkiaapa, Lapland, Finland</t>
+  </si>
+  <si>
+    <t>Tero Linjama</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/YSDNMROVID</t>
+  </si>
+  <si>
+    <t>Calidris ferruginea</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/346641/download</t>
+  </si>
+  <si>
+    <t>Walvisbay, Namibia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/184321/download</t>
+  </si>
+  <si>
+    <t>Kazaly District, Kyzylorda Province, Kazakhstan</t>
+  </si>
+  <si>
+    <t>Albert Lastukhin</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/LELYWQKUZX</t>
+  </si>
+  <si>
+    <t>Calidris melanotos</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/406470/download</t>
+  </si>
+  <si>
+    <t>Barrow, Alaksa, United States</t>
+  </si>
+  <si>
+    <t>Calidris ruficollis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/107881/download</t>
+  </si>
+  <si>
+    <t>Monkey Mia, Western Australia, Australia</t>
+  </si>
+  <si>
+    <t>Calidris subminuta</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/295966/download</t>
+  </si>
+  <si>
+    <t>Dalian, China</t>
+  </si>
+  <si>
+    <t>Tom Beeke</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/CTULRNLZWS</t>
+  </si>
+  <si>
+    <t>Calidris subruficollis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/435877/download</t>
+  </si>
+  <si>
+    <t>Calidris tenuirostris</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/396375/download</t>
+  </si>
+  <si>
+    <t>Trevozhnaya, Chukotka Autonomous Okrug, Russian Federation</t>
+  </si>
+  <si>
+    <t>Christian A. Jensen</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/IBLQAJNUOV</t>
+  </si>
+  <si>
+    <t>Caligavis chrysops</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/390581/download</t>
+  </si>
+  <si>
+    <t>Burralow Creek, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/104876/download</t>
+  </si>
+  <si>
+    <t>Mogo Creek, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Eliot Miller</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/YLVIJORHMB</t>
+  </si>
+  <si>
+    <t>Calyptorhynchus banksii</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/439665/download</t>
+  </si>
+  <si>
+    <t>Twin Bridges, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/104983/download</t>
   </si>
 </sst>
 </file>
@@ -1152,11 +1464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,6 +3297,857 @@
         <v>28</v>
       </c>
     </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>256</v>
+      </c>
+      <c r="B80" t="s">
+        <v>257</v>
+      </c>
+      <c r="C80" t="s">
+        <v>258</v>
+      </c>
+      <c r="D80" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>259</v>
+      </c>
+      <c r="B81" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" t="s">
+        <v>261</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" t="s">
+        <v>27</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>262</v>
+      </c>
+      <c r="B82" t="s">
+        <v>263</v>
+      </c>
+      <c r="C82" t="s">
+        <v>264</v>
+      </c>
+      <c r="D82" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" t="s">
+        <v>265</v>
+      </c>
+      <c r="C83" t="s">
+        <v>266</v>
+      </c>
+      <c r="D83" t="s">
+        <v>31</v>
+      </c>
+      <c r="E83" t="s">
+        <v>32</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>262</v>
+      </c>
+      <c r="B84" t="s">
+        <v>267</v>
+      </c>
+      <c r="C84" t="s">
+        <v>268</v>
+      </c>
+      <c r="D84" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" t="s">
+        <v>32</v>
+      </c>
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>269</v>
+      </c>
+      <c r="B85" t="s">
+        <v>270</v>
+      </c>
+      <c r="C85" t="s">
+        <v>271</v>
+      </c>
+      <c r="D85" t="s">
+        <v>197</v>
+      </c>
+      <c r="E85" t="s">
+        <v>198</v>
+      </c>
+      <c r="F85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>269</v>
+      </c>
+      <c r="B86" t="s">
+        <v>272</v>
+      </c>
+      <c r="C86" t="s">
+        <v>273</v>
+      </c>
+      <c r="D86" t="s">
+        <v>75</v>
+      </c>
+      <c r="E86" t="s">
+        <v>76</v>
+      </c>
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>274</v>
+      </c>
+      <c r="B87" t="s">
+        <v>275</v>
+      </c>
+      <c r="C87" t="s">
+        <v>253</v>
+      </c>
+      <c r="D87" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" t="s">
+        <v>276</v>
+      </c>
+      <c r="C88" t="s">
+        <v>277</v>
+      </c>
+      <c r="D88" t="s">
+        <v>26</v>
+      </c>
+      <c r="E88" t="s">
+        <v>27</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>278</v>
+      </c>
+      <c r="B89" t="s">
+        <v>279</v>
+      </c>
+      <c r="C89" t="s">
+        <v>280</v>
+      </c>
+      <c r="D89" t="s">
+        <v>84</v>
+      </c>
+      <c r="E89" t="s">
+        <v>85</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>278</v>
+      </c>
+      <c r="B90" t="s">
+        <v>281</v>
+      </c>
+      <c r="C90" t="s">
+        <v>282</v>
+      </c>
+      <c r="D90" t="s">
+        <v>75</v>
+      </c>
+      <c r="E90" t="s">
+        <v>76</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>283</v>
+      </c>
+      <c r="B91" t="s">
+        <v>284</v>
+      </c>
+      <c r="C91" t="s">
+        <v>285</v>
+      </c>
+      <c r="D91" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" t="s">
+        <v>32</v>
+      </c>
+      <c r="F91" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>283</v>
+      </c>
+      <c r="B92" t="s">
+        <v>286</v>
+      </c>
+      <c r="C92" t="s">
+        <v>287</v>
+      </c>
+      <c r="D92" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" t="s">
+        <v>76</v>
+      </c>
+      <c r="F92" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>288</v>
+      </c>
+      <c r="B93" t="s">
+        <v>289</v>
+      </c>
+      <c r="C93" t="s">
+        <v>142</v>
+      </c>
+      <c r="D93" t="s">
+        <v>84</v>
+      </c>
+      <c r="E93" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>288</v>
+      </c>
+      <c r="B94" t="s">
+        <v>290</v>
+      </c>
+      <c r="C94" t="s">
+        <v>291</v>
+      </c>
+      <c r="D94" t="s">
+        <v>31</v>
+      </c>
+      <c r="E94" t="s">
+        <v>32</v>
+      </c>
+      <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>288</v>
+      </c>
+      <c r="B95" t="s">
+        <v>292</v>
+      </c>
+      <c r="C95" t="s">
+        <v>293</v>
+      </c>
+      <c r="D95" t="s">
+        <v>31</v>
+      </c>
+      <c r="E95" t="s">
+        <v>32</v>
+      </c>
+      <c r="F95" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>294</v>
+      </c>
+      <c r="B96" t="s">
+        <v>295</v>
+      </c>
+      <c r="C96" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" t="s">
+        <v>31</v>
+      </c>
+      <c r="E96" t="s">
+        <v>32</v>
+      </c>
+      <c r="F96" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>294</v>
+      </c>
+      <c r="B97" t="s">
+        <v>296</v>
+      </c>
+      <c r="C97" t="s">
+        <v>250</v>
+      </c>
+      <c r="D97" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" t="s">
+        <v>32</v>
+      </c>
+      <c r="F97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>297</v>
+      </c>
+      <c r="B98" t="s">
+        <v>298</v>
+      </c>
+      <c r="C98" t="s">
+        <v>299</v>
+      </c>
+      <c r="D98" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" t="s">
+        <v>32</v>
+      </c>
+      <c r="F98" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>297</v>
+      </c>
+      <c r="B99" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F99" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" t="s">
+        <v>302</v>
+      </c>
+      <c r="C100" t="s">
+        <v>303</v>
+      </c>
+      <c r="D100" t="s">
+        <v>304</v>
+      </c>
+      <c r="E100" t="s">
+        <v>305</v>
+      </c>
+      <c r="F100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>301</v>
+      </c>
+      <c r="B101" t="s">
+        <v>306</v>
+      </c>
+      <c r="C101" t="s">
+        <v>237</v>
+      </c>
+      <c r="D101" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" t="s">
+        <v>32</v>
+      </c>
+      <c r="F101" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>307</v>
+      </c>
+      <c r="B102" t="s">
+        <v>308</v>
+      </c>
+      <c r="C102" t="s">
+        <v>309</v>
+      </c>
+      <c r="D102" t="s">
+        <v>84</v>
+      </c>
+      <c r="E102" t="s">
+        <v>85</v>
+      </c>
+      <c r="F102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>307</v>
+      </c>
+      <c r="B103" t="s">
+        <v>310</v>
+      </c>
+      <c r="C103" t="s">
+        <v>311</v>
+      </c>
+      <c r="D103" t="s">
+        <v>312</v>
+      </c>
+      <c r="E103" t="s">
+        <v>313</v>
+      </c>
+      <c r="F103" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>314</v>
+      </c>
+      <c r="B104" t="s">
+        <v>315</v>
+      </c>
+      <c r="C104" t="s">
+        <v>316</v>
+      </c>
+      <c r="D104" t="s">
+        <v>318</v>
+      </c>
+      <c r="E104" t="s">
+        <v>317</v>
+      </c>
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>319</v>
+      </c>
+      <c r="B105" t="s">
+        <v>320</v>
+      </c>
+      <c r="C105" t="s">
+        <v>321</v>
+      </c>
+      <c r="D105" t="s">
+        <v>322</v>
+      </c>
+      <c r="E105" t="s">
+        <v>323</v>
+      </c>
+      <c r="F105" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>324</v>
+      </c>
+      <c r="B106" t="s">
+        <v>325</v>
+      </c>
+      <c r="C106" t="s">
+        <v>326</v>
+      </c>
+      <c r="D106" t="s">
+        <v>197</v>
+      </c>
+      <c r="E106" t="s">
+        <v>198</v>
+      </c>
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>324</v>
+      </c>
+      <c r="B107" t="s">
+        <v>327</v>
+      </c>
+      <c r="C107" t="s">
+        <v>328</v>
+      </c>
+      <c r="D107" t="s">
+        <v>329</v>
+      </c>
+      <c r="E107" t="s">
+        <v>330</v>
+      </c>
+      <c r="F107" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>331</v>
+      </c>
+      <c r="B108" t="s">
+        <v>332</v>
+      </c>
+      <c r="C108" t="s">
+        <v>333</v>
+      </c>
+      <c r="D108" t="s">
+        <v>114</v>
+      </c>
+      <c r="E108" t="s">
+        <v>115</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>334</v>
+      </c>
+      <c r="B109" t="s">
+        <v>335</v>
+      </c>
+      <c r="C109" t="s">
+        <v>336</v>
+      </c>
+      <c r="D109" t="s">
+        <v>89</v>
+      </c>
+      <c r="E109" t="s">
+        <v>90</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>337</v>
+      </c>
+      <c r="B110" t="s">
+        <v>338</v>
+      </c>
+      <c r="C110" t="s">
+        <v>339</v>
+      </c>
+      <c r="D110" t="s">
+        <v>340</v>
+      </c>
+      <c r="E110" t="s">
+        <v>341</v>
+      </c>
+      <c r="F110" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>342</v>
+      </c>
+      <c r="B111" t="s">
+        <v>343</v>
+      </c>
+      <c r="C111" t="s">
+        <v>203</v>
+      </c>
+      <c r="D111" t="s">
+        <v>204</v>
+      </c>
+      <c r="E111" t="s">
+        <v>205</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>344</v>
+      </c>
+      <c r="B112" t="s">
+        <v>345</v>
+      </c>
+      <c r="C112" t="s">
+        <v>346</v>
+      </c>
+      <c r="D112" t="s">
+        <v>347</v>
+      </c>
+      <c r="E112" t="s">
+        <v>348</v>
+      </c>
+      <c r="F112" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>349</v>
+      </c>
+      <c r="B113" t="s">
+        <v>350</v>
+      </c>
+      <c r="C113" t="s">
+        <v>351</v>
+      </c>
+      <c r="D113" t="s">
+        <v>31</v>
+      </c>
+      <c r="E113" t="s">
+        <v>32</v>
+      </c>
+      <c r="F113" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>349</v>
+      </c>
+      <c r="B114" t="s">
+        <v>352</v>
+      </c>
+      <c r="C114" t="s">
+        <v>353</v>
+      </c>
+      <c r="D114" t="s">
+        <v>354</v>
+      </c>
+      <c r="E114" t="s">
+        <v>355</v>
+      </c>
+      <c r="F114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>356</v>
+      </c>
+      <c r="B115" t="s">
+        <v>357</v>
+      </c>
+      <c r="C115" t="s">
+        <v>358</v>
+      </c>
+      <c r="D115" t="s">
+        <v>31</v>
+      </c>
+      <c r="E115" t="s">
+        <v>32</v>
+      </c>
+      <c r="F115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>356</v>
+      </c>
+      <c r="B116" t="s">
+        <v>359</v>
+      </c>
+      <c r="C116" t="s">
+        <v>154</v>
+      </c>
+      <c r="D116" t="s">
+        <v>354</v>
+      </c>
+      <c r="E116" t="s">
+        <v>355</v>
+      </c>
+      <c r="F116" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:G50">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
dozen more audio files
</commit_message>
<xml_diff>
--- a/data/audio/audio.xlsx
+++ b/data/audio/audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B26E46-43A7-4858-A0CE-A8120AE47BB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BD2068-E4D8-4016-8F45-CDC18A67C0B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="482">
   <si>
     <t>species_scientific_name</t>
   </si>
@@ -1354,6 +1354,123 @@
   </si>
   <si>
     <t>https://ebird.org/profile/NDU3MzMz</t>
+  </si>
+  <si>
+    <t>Circus approximans</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/153004/download</t>
+  </si>
+  <si>
+    <t>Christchurch, New Zealand</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/153003/download</t>
+  </si>
+  <si>
+    <t>Circus assimilis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/194155/download</t>
+  </si>
+  <si>
+    <t>Toraut, Sulawesi, Indonesia</t>
+  </si>
+  <si>
+    <t>Cisticola exilis</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/59528/download</t>
+  </si>
+  <si>
+    <t>Lake Samsonvale, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Peter Woodall</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/SILWLBBIFA</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/389373/download</t>
+  </si>
+  <si>
+    <t>Climacteris erythrops</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/172242/download</t>
+  </si>
+  <si>
+    <t>Newnes Plateau, New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/98376/download</t>
+  </si>
+  <si>
+    <t>Lamington National Park, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Climacteris picumnus</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/343748/download</t>
+  </si>
+  <si>
+    <t>Cunnamulla, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/334462/download</t>
+  </si>
+  <si>
+    <t>Gluepot Reserve, South Australia, Australia</t>
+  </si>
+  <si>
+    <t>Colluricincla harmonica</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/210922/download</t>
+  </si>
+  <si>
+    <t>Gold Creek Reservoir, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Mike Williamson</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/PFQCEGABBH</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/434562/download</t>
+  </si>
+  <si>
+    <t>Mount Moffat, Queensland, Australia</t>
+  </si>
+  <si>
+    <t>Colluricincla megarhyncha</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/349118/download</t>
+  </si>
+  <si>
+    <t>Columba leucomela</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/351946/download</t>
+  </si>
+  <si>
+    <t>Columba livia</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/462661/download</t>
+  </si>
+  <si>
+    <t>Gmina Hańsk, Lublin Voivodeship, Poland</t>
+  </si>
+  <si>
+    <t>Stanislas Wroza</t>
+  </si>
+  <si>
+    <t>https://www.xeno-canto.org/contributor/SDPCHKOHRH</t>
   </si>
 </sst>
 </file>
@@ -1713,11 +1830,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5176,6 +5293,328 @@
         <v>54</v>
       </c>
     </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>443</v>
+      </c>
+      <c r="B151" t="s">
+        <v>444</v>
+      </c>
+      <c r="C151" t="s">
+        <v>445</v>
+      </c>
+      <c r="D151" t="s">
+        <v>44</v>
+      </c>
+      <c r="E151" t="s">
+        <v>45</v>
+      </c>
+      <c r="F151" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>443</v>
+      </c>
+      <c r="B152" t="s">
+        <v>446</v>
+      </c>
+      <c r="C152" t="s">
+        <v>445</v>
+      </c>
+      <c r="D152" t="s">
+        <v>44</v>
+      </c>
+      <c r="E152" t="s">
+        <v>45</v>
+      </c>
+      <c r="F152" t="s">
+        <v>12</v>
+      </c>
+      <c r="G152" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>447</v>
+      </c>
+      <c r="B153" t="s">
+        <v>448</v>
+      </c>
+      <c r="C153" t="s">
+        <v>449</v>
+      </c>
+      <c r="D153" t="s">
+        <v>84</v>
+      </c>
+      <c r="E153" t="s">
+        <v>85</v>
+      </c>
+      <c r="F153" t="s">
+        <v>12</v>
+      </c>
+      <c r="G153" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>450</v>
+      </c>
+      <c r="B154" t="s">
+        <v>451</v>
+      </c>
+      <c r="C154" t="s">
+        <v>452</v>
+      </c>
+      <c r="D154" t="s">
+        <v>453</v>
+      </c>
+      <c r="E154" t="s">
+        <v>454</v>
+      </c>
+      <c r="F154" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>450</v>
+      </c>
+      <c r="B155" t="s">
+        <v>455</v>
+      </c>
+      <c r="C155" t="s">
+        <v>250</v>
+      </c>
+      <c r="D155" t="s">
+        <v>31</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F155" t="s">
+        <v>12</v>
+      </c>
+      <c r="G155" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>456</v>
+      </c>
+      <c r="B156" t="s">
+        <v>457</v>
+      </c>
+      <c r="C156" t="s">
+        <v>458</v>
+      </c>
+      <c r="D156" t="s">
+        <v>31</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F156" t="s">
+        <v>12</v>
+      </c>
+      <c r="G156" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>456</v>
+      </c>
+      <c r="B157" t="s">
+        <v>459</v>
+      </c>
+      <c r="C157" t="s">
+        <v>460</v>
+      </c>
+      <c r="D157" t="s">
+        <v>114</v>
+      </c>
+      <c r="E157" t="s">
+        <v>115</v>
+      </c>
+      <c r="F157" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>461</v>
+      </c>
+      <c r="B158" t="s">
+        <v>462</v>
+      </c>
+      <c r="C158" t="s">
+        <v>463</v>
+      </c>
+      <c r="D158" t="s">
+        <v>26</v>
+      </c>
+      <c r="E158" t="s">
+        <v>27</v>
+      </c>
+      <c r="F158" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>461</v>
+      </c>
+      <c r="B159" t="s">
+        <v>464</v>
+      </c>
+      <c r="C159" t="s">
+        <v>465</v>
+      </c>
+      <c r="D159" t="s">
+        <v>31</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F159" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>466</v>
+      </c>
+      <c r="B160" t="s">
+        <v>467</v>
+      </c>
+      <c r="C160" t="s">
+        <v>468</v>
+      </c>
+      <c r="D160" t="s">
+        <v>469</v>
+      </c>
+      <c r="E160" t="s">
+        <v>470</v>
+      </c>
+      <c r="F160" t="s">
+        <v>12</v>
+      </c>
+      <c r="G160" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>466</v>
+      </c>
+      <c r="B161" t="s">
+        <v>471</v>
+      </c>
+      <c r="C161" t="s">
+        <v>472</v>
+      </c>
+      <c r="D161" t="s">
+        <v>31</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F161" t="s">
+        <v>12</v>
+      </c>
+      <c r="G161" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>473</v>
+      </c>
+      <c r="B162" t="s">
+        <v>474</v>
+      </c>
+      <c r="C162" t="s">
+        <v>261</v>
+      </c>
+      <c r="D162" t="s">
+        <v>31</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F162" t="s">
+        <v>12</v>
+      </c>
+      <c r="G162" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>475</v>
+      </c>
+      <c r="B163" t="s">
+        <v>476</v>
+      </c>
+      <c r="C163" t="s">
+        <v>460</v>
+      </c>
+      <c r="D163" t="s">
+        <v>26</v>
+      </c>
+      <c r="E163" t="s">
+        <v>27</v>
+      </c>
+      <c r="F163" t="s">
+        <v>12</v>
+      </c>
+      <c r="G163" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>477</v>
+      </c>
+      <c r="B164" t="s">
+        <v>478</v>
+      </c>
+      <c r="C164" t="s">
+        <v>479</v>
+      </c>
+      <c r="D164" t="s">
+        <v>480</v>
+      </c>
+      <c r="E164" t="s">
+        <v>481</v>
+      </c>
+      <c r="F164" t="s">
+        <v>12</v>
+      </c>
+      <c r="G164" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:G50">
     <sortCondition ref="A1"/>

</xml_diff>